<commit_message>
Muharrem - Test Case Update
</commit_message>
<xml_diff>
--- a/src/test/java/Resources/SamsungTestCases.xlsx
+++ b/src/test/java/Resources/SamsungTestCases.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkara\IdeaProjects\Samsung\src\test\java\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7668"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
   <si>
     <t>TestID</t>
   </si>
@@ -219,13 +224,100 @@
   </si>
   <si>
     <t>The User should be able to close open pages</t>
+  </si>
+  <si>
+    <t>Muharrem Karapazar</t>
+  </si>
+  <si>
+    <t>The warranty period given by the company to the products should match the warranty periods on the website.</t>
+  </si>
+  <si>
+    <t>4.Go to Samsung support page</t>
+  </si>
+  <si>
+    <t>5.Click on LEARN MORE to see warranty terms</t>
+  </si>
+  <si>
+    <t>6.Compare the warranty period of mobile devices with data</t>
+  </si>
+  <si>
+    <t>7.Compare the warranty period of TV and Lighting devices with the data</t>
+  </si>
+  <si>
+    <t>8.Compare the warranty period of WHITE GOODS with the data</t>
+  </si>
+  <si>
+    <t>9.Compare the warranty period of COMPUTER AND OFFICE devices with the data</t>
+  </si>
+  <si>
+    <t>10.Compare the warranty period of CAMERA AND VIDEO CAMERA devices with data</t>
+  </si>
+  <si>
+    <t>11.Compare the warranty period of the STORAGE devices with the data</t>
+  </si>
+  <si>
+    <t>And Click on LEARN MORE to see warranty terms</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of mobile devices with data</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of TV and Lighting devices with the data</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of WHITE GOODS with the data</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of COMPUTER AND OFFICE devices with the data</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of CAMERA AND VIDEO CAMERA devices with data</t>
+  </si>
+  <si>
+    <t>And Compare the warranty period of the STORAGE devices with the data</t>
+  </si>
+  <si>
+    <t>And Close cookie window</t>
+  </si>
+  <si>
+    <t>When Get successfully message Samsung</t>
+  </si>
+  <si>
+    <t>And Go to Samsung support page</t>
+  </si>
+  <si>
+    <t>Then Close open pages</t>
+  </si>
+  <si>
+    <t>You should be able to go to the Samsung support page.</t>
+  </si>
+  <si>
+    <t>You should be able to click the MORE INFORMATION link to see the warranty terms.</t>
+  </si>
+  <si>
+    <t>The warranty period of mobile devices should be clearly visible.</t>
+  </si>
+  <si>
+    <t>The warranty period of TV and Lighting devices should be clearly visible.</t>
+  </si>
+  <si>
+    <t>The warranty period of WHITE GOODS devices should be clearly visible.</t>
+  </si>
+  <si>
+    <t>The warranty period of COMPUTER AND OFFICE devices should be clearly visible.</t>
+  </si>
+  <si>
+    <t>The warranty period of CAMERA AND VIDEO CAMERA devices should be clearly visible.</t>
+  </si>
+  <si>
+    <t>The warranty period of the STORAGE devices must be clearly visible.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,7 +463,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1497138</xdr:colOff>
+      <xdr:colOff>773238</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>67163</xdr:rowOff>
     </xdr:to>
@@ -446,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -481,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -658,35 +750,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="65.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="83.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="85.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="94" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -715,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="47.25" customHeight="1">
+    <row r="2" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -744,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
@@ -759,7 +851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1">
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8" t="s">
         <v>31</v>
       </c>
@@ -767,129 +859,129 @@
       <c r="G4" s="8"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75">
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75">
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E16" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.75" customHeight="1">
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E20" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E28" s="2"/>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1">
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -900,7 +992,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="75.75">
+    <row r="31" spans="1:9" ht="75.599999999999994" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -929,7 +1021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E32" s="2" t="s">
         <v>15</v>
       </c>
@@ -942,7 +1034,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="5:9" ht="15.75">
+    <row r="33" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E33" s="8" t="s">
         <v>31</v>
       </c>
@@ -955,7 +1047,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="5:9" ht="15.75">
+    <row r="34" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E34" s="2" t="s">
         <v>49</v>
       </c>
@@ -967,7 +1059,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="5:9" ht="15.75">
+    <row r="35" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>50</v>
       </c>
@@ -979,7 +1071,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="5:9" ht="15.75">
+    <row r="36" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>51</v>
       </c>
@@ -991,7 +1083,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="5:9" ht="15.75">
+    <row r="37" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E37" s="2" t="s">
         <v>52</v>
       </c>
@@ -1003,7 +1095,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="5:9" ht="15.75">
+    <row r="38" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E38" s="2" t="s">
         <v>53</v>
       </c>
@@ -1015,7 +1107,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="5:9" ht="15.75">
+    <row r="39" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E39" s="2" t="s">
         <v>54</v>
       </c>
@@ -1027,7 +1119,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="5:9" ht="15.75">
+    <row r="40" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E40" s="2" t="s">
         <v>55</v>
       </c>
@@ -1039,85 +1131,85 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="5:9" ht="15.75">
+    <row r="41" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="5:9" ht="15.75">
+    <row r="42" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="44" spans="5:9" ht="15.75">
+    <row r="44" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="5:9" ht="15.75">
+    <row r="45" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E45" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="5:9" ht="15.75">
+    <row r="46" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E46" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="5:9" ht="15.75">
+    <row r="47" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E47" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="5:9" ht="15.75">
+    <row r="48" spans="5:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E48" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E49" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E50" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E51" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E52" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E53" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E54" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E55" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E56" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:9" s="5" customFormat="1">
+    <row r="58" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1128,24 +1220,216 @@
       <c r="H58" s="3"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75">
+    <row r="59" spans="1:9" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="E59" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F59" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" s="5" customFormat="1">
+      <c r="G59" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E61" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E63" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E64" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E65" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E66" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E68" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E69" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E71" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E72" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E73" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E74" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E75" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E76" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E77" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E78" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E79" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E80" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E81" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E82" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E83" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E84" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1156,7 +1440,7 @@
       <c r="H85" s="3"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" spans="1:9" ht="15.75">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="5" customFormat="1">
+    <row r="120" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -1184,7 +1468,7 @@
       <c r="H120" s="3"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="1:9" ht="15.75">
+    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>18</v>
       </c>
@@ -1201,7 +1485,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:9" s="5" customFormat="1">
+    <row r="155" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -1212,7 +1496,7 @@
       <c r="H155" s="3"/>
       <c r="I155" s="4"/>
     </row>
-    <row r="156" spans="1:9" ht="15.75">
+    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>